<commit_message>
new format and script
</commit_message>
<xml_diff>
--- a/newformat_data/05_Maio_-_Itamar.xlsx
+++ b/newformat_data/05_Maio_-_Itamar.xlsx
@@ -2068,9 +2068,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>728640</xdr:colOff>
+      <xdr:colOff>728280</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2084,7 +2084,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="76320"/>
-          <a:ext cx="1455480" cy="1293120"/>
+          <a:ext cx="1455120" cy="1292760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2110,9 +2110,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2126,7 +2126,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="76320"/>
-          <a:ext cx="1455120" cy="1293120"/>
+          <a:ext cx="1454760" cy="1292760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2152,9 +2152,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2168,7 +2168,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="76320"/>
-          <a:ext cx="1455120" cy="1293120"/>
+          <a:ext cx="1454760" cy="1292760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2194,9 +2194,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2210,7 +2210,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="76320"/>
-          <a:ext cx="1455120" cy="1293120"/>
+          <a:ext cx="1454760" cy="1292760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2236,9 +2236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2252,7 +2252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="76320"/>
-          <a:ext cx="1455120" cy="1293120"/>
+          <a:ext cx="1454760" cy="1292760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2278,9 +2278,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2294,7 +2294,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="76320"/>
-          <a:ext cx="1455120" cy="1293120"/>
+          <a:ext cx="1454760" cy="1292760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2320,9 +2320,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2336,7 +2336,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="76320"/>
-          <a:ext cx="1455120" cy="1293120"/>
+          <a:ext cx="1454760" cy="1292760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2362,9 +2362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2378,7 +2378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="76320"/>
-          <a:ext cx="1455120" cy="1293120"/>
+          <a:ext cx="1454760" cy="1292760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2401,7 +2401,7 @@
   <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>